<commit_message>
Added navX library and worked on drives
</commit_message>
<xml_diff>
--- a/Check Sheets/DistanceperTick.xlsx
+++ b/Check Sheets/DistanceperTick.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FRC2019\Check Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DAFE086-7011-40EA-BE64-52F38D0E4E1E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2401DB1-CF64-4EC9-A36F-67778AE1B154}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11003" xr2:uid="{3263B50B-037C-4109-801E-E9732B8A4E3D}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>countsPerCycle</t>
   </si>
@@ -40,13 +39,25 @@
     <t>circOfWheel</t>
   </si>
   <si>
-    <t>GearRatio</t>
-  </si>
-  <si>
     <t>Inches</t>
   </si>
   <si>
     <t>Output</t>
+  </si>
+  <si>
+    <t>GearRatio to Encoder</t>
+  </si>
+  <si>
+    <t>GearRatio to Motor</t>
+  </si>
+  <si>
+    <t>Max RPM</t>
+  </si>
+  <si>
+    <t>counts per 100ms At Max</t>
+  </si>
+  <si>
+    <t>Ticks per rev</t>
   </si>
 </sst>
 </file>
@@ -398,15 +409,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3D60F3-4D31-49A5-9299-4FEF4360D502}">
-  <dimension ref="A2:B7"/>
+  <dimension ref="A2:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.265625" customWidth="1"/>
+    <col min="1" max="1" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
@@ -428,7 +439,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <f>(54/28)*(22/12)</f>
@@ -437,7 +448,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -445,11 +456,46 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7">
         <f>TRUNC(B6*(B4*B2/B3))</f>
         <v>2813</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <f>40/20</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <f>B2/B9</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <f>B11/600*B12</f>
+        <v>4833.333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>